<commit_message>
Finished data from Alabama to Kentucky
</commit_message>
<xml_diff>
--- a/data-v2.xlsx
+++ b/data-v2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
   <si>
     <t>state</t>
   </si>
@@ -262,7 +262,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,47 +873,401 @@
       <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="B7">
+        <v>48</v>
+      </c>
+      <c r="C7" s="1">
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>77</v>
+      </c>
+      <c r="G7">
+        <v>18</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>12</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>33</v>
+      </c>
+      <c r="M7">
+        <v>14</v>
+      </c>
+      <c r="N7">
+        <v>44</v>
+      </c>
+      <c r="O7">
+        <v>4</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>39</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>18</v>
+      </c>
+      <c r="M8">
+        <v>12</v>
+      </c>
+      <c r="N8">
+        <v>27</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>66</v>
+      </c>
+      <c r="M9" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
+      <c r="B10">
+        <v>302</v>
+      </c>
+      <c r="C10" s="1">
+        <v>68</v>
+      </c>
+      <c r="D10">
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <v>24</v>
+      </c>
+      <c r="F10">
+        <v>407</v>
+      </c>
+      <c r="G10">
+        <v>63</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <v>37</v>
+      </c>
+      <c r="J10">
+        <v>40</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>206</v>
+      </c>
+      <c r="M10">
+        <v>99</v>
+      </c>
+      <c r="N10">
+        <v>282</v>
+      </c>
+      <c r="O10">
+        <v>9</v>
+      </c>
+      <c r="P10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="B11">
+        <v>151</v>
+      </c>
+      <c r="C11" s="1">
+        <v>26</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>191</v>
+      </c>
+      <c r="G11">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11">
+        <v>9</v>
+      </c>
+      <c r="J11">
+        <v>19</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>106</v>
+      </c>
+      <c r="M11">
+        <v>48</v>
+      </c>
+      <c r="N11">
+        <v>144</v>
+      </c>
+      <c r="O11">
+        <v>3</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="B12">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>17</v>
+      </c>
+      <c r="M12">
+        <v>6</v>
+      </c>
+      <c r="N12">
+        <v>21</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="M13" t="s">
+        <v>66</v>
+      </c>
+      <c r="N13">
+        <v>5</v>
+      </c>
+      <c r="O13" t="s">
+        <v>66</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="B14">
+        <v>92</v>
+      </c>
+      <c r="C14" s="1">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>122</v>
+      </c>
+      <c r="G14">
+        <v>22</v>
+      </c>
+      <c r="H14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14">
+        <v>12</v>
+      </c>
+      <c r="J14">
+        <v>12</v>
+      </c>
+      <c r="K14" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14">
+        <v>68</v>
+      </c>
+      <c r="M14">
+        <v>27</v>
+      </c>
+      <c r="N14">
+        <v>84</v>
+      </c>
+      <c r="O14">
+        <v>3</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -969,191 +1323,349 @@
       <c r="A16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>36</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>66</v>
+      </c>
+      <c r="J16" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>20</v>
+      </c>
+      <c r="M16">
+        <v>6</v>
+      </c>
+      <c r="N16">
+        <v>23</v>
+      </c>
+      <c r="O16">
+        <v>3</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>31</v>
+      </c>
+      <c r="C17" s="1">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>43</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>19</v>
+      </c>
+      <c r="M17">
+        <v>14</v>
+      </c>
+      <c r="N17">
+        <v>28</v>
+      </c>
+      <c r="O17" t="s">
+        <v>66</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>45</v>
+      </c>
+      <c r="C18" s="1">
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>6</v>
+      </c>
+      <c r="F18">
+        <v>63</v>
+      </c>
+      <c r="G18">
+        <v>6</v>
+      </c>
+      <c r="H18" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>28</v>
+      </c>
+      <c r="M18">
+        <v>19</v>
+      </c>
+      <c r="N18">
+        <v>41</v>
+      </c>
+      <c r="O18">
+        <v>3</v>
+      </c>
+      <c r="P18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>40</v>
       </c>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>65</v>
       </c>
+      <c r="C51" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
My Data Added - Ohio to Wyoming
</commit_message>
<xml_diff>
--- a/data-v2.xlsx
+++ b/data-v2.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brad Cardello\Desktop\Computer Science\CMPS-165\Human Trafficking Project\human-trafficking-visualization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/douglasws89/Desktop/human-trafficking-visualization/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500"/>
   </bookViews>
   <sheets>
     <sheet name="data-v1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="67">
   <si>
     <t>state</t>
   </si>
@@ -326,9 +329,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -361,9 +364,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -545,31 +548,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="7.5" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.5" customWidth="1"/>
+    <col min="12" max="12" width="9.83203125" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" customWidth="1"/>
+    <col min="15" max="16" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -619,7 +621,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -669,7 +671,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -719,7 +721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -769,7 +771,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -819,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -869,7 +871,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -919,7 +921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -969,7 +971,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1019,7 +1021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1069,7 +1071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1119,7 +1121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1169,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1219,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1269,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1319,7 +1321,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1369,7 +1371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1419,7 +1421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1469,203 +1471,994 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>57</v>
+      </c>
+      <c r="C19" s="1">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>75</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19">
+        <v>8</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>31</v>
+      </c>
+      <c r="M19">
+        <v>21</v>
+      </c>
+      <c r="N19">
+        <v>51</v>
+      </c>
+      <c r="O19" t="s">
+        <v>66</v>
+      </c>
+      <c r="P19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>10</v>
+      </c>
+      <c r="G20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>66</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>3</v>
+      </c>
+      <c r="M20" t="s">
+        <v>66</v>
+      </c>
+      <c r="N20">
+        <v>6</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>38</v>
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>40</v>
       </c>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>41</v>
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>42</v>
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>43</v>
       </c>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>44</v>
       </c>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>45</v>
       </c>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>46</v>
       </c>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>47</v>
       </c>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>48</v>
       </c>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>233</v>
+      </c>
+      <c r="C36" s="1">
+        <v>18</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="E36">
+        <v>30</v>
+      </c>
+      <c r="F36">
+        <v>289</v>
+      </c>
+      <c r="G36">
+        <v>14</v>
+      </c>
+      <c r="H36">
+        <v>4</v>
+      </c>
+      <c r="I36">
+        <v>12</v>
+      </c>
+      <c r="J36">
+        <v>6</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>172</v>
+      </c>
+      <c r="M36">
+        <v>53</v>
+      </c>
+      <c r="N36">
+        <v>218</v>
+      </c>
+      <c r="O36">
+        <v>8</v>
+      </c>
+      <c r="P36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>28</v>
+      </c>
+      <c r="C37" s="1">
+        <v>9</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>42</v>
+      </c>
+      <c r="G37">
+        <v>9</v>
+      </c>
+      <c r="H37" t="s">
+        <v>66</v>
+      </c>
+      <c r="I37">
+        <v>5</v>
+      </c>
+      <c r="J37">
+        <v>6</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>18</v>
+      </c>
+      <c r="M37">
+        <v>10</v>
+      </c>
+      <c r="N37">
+        <v>27</v>
+      </c>
+      <c r="O37" t="s">
+        <v>66</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>44</v>
+      </c>
+      <c r="C38" s="1">
+        <v>8</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="F38">
+        <v>56</v>
+      </c>
+      <c r="G38">
+        <v>6</v>
+      </c>
+      <c r="H38" t="s">
+        <v>66</v>
+      </c>
+      <c r="I38">
+        <v>7</v>
+      </c>
+      <c r="J38" t="s">
+        <v>66</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>32</v>
+      </c>
+      <c r="M38">
+        <v>11</v>
+      </c>
+      <c r="N38">
+        <v>42</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>80</v>
+      </c>
+      <c r="C39" s="1">
+        <v>15</v>
+      </c>
+      <c r="D39">
+        <v>6</v>
+      </c>
+      <c r="E39">
+        <v>5</v>
+      </c>
+      <c r="F39">
+        <v>106</v>
+      </c>
+      <c r="G39">
+        <v>14</v>
+      </c>
+      <c r="H39" t="s">
+        <v>66</v>
+      </c>
+      <c r="I39">
+        <v>9</v>
+      </c>
+      <c r="J39">
+        <v>7</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <v>53</v>
+      </c>
+      <c r="M39">
+        <v>20</v>
+      </c>
+      <c r="N39">
+        <v>68</v>
+      </c>
+      <c r="O39">
+        <v>4</v>
+      </c>
+      <c r="P39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>8</v>
+      </c>
+      <c r="G40" t="s">
+        <v>66</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40" t="s">
+        <v>66</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>5</v>
+      </c>
+      <c r="M40" t="s">
+        <v>66</v>
+      </c>
+      <c r="N40">
+        <v>5</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>42</v>
+      </c>
+      <c r="C41" s="1">
+        <v>14</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41">
+        <v>61</v>
+      </c>
+      <c r="G41">
+        <v>13</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>6</v>
+      </c>
+      <c r="J41">
+        <v>11</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>26</v>
+      </c>
+      <c r="M41">
+        <v>22</v>
+      </c>
+      <c r="N41">
+        <v>39</v>
+      </c>
+      <c r="O41">
+        <v>3</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>56</v>
       </c>
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>9</v>
+      </c>
+      <c r="C42" s="1">
+        <v>5</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>15</v>
+      </c>
+      <c r="G42">
+        <v>4</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>4</v>
+      </c>
+      <c r="J42" t="s">
+        <v>66</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>6</v>
+      </c>
+      <c r="M42">
+        <v>3</v>
+      </c>
+      <c r="N42">
+        <v>9</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>53</v>
+      </c>
+      <c r="C43" s="1">
+        <v>12</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <v>69</v>
+      </c>
+      <c r="G43">
+        <v>10</v>
+      </c>
+      <c r="H43" t="s">
+        <v>66</v>
+      </c>
+      <c r="I43">
+        <v>6</v>
+      </c>
+      <c r="J43">
+        <v>7</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>28</v>
+      </c>
+      <c r="M43">
+        <v>23</v>
+      </c>
+      <c r="N43">
+        <v>51</v>
+      </c>
+      <c r="O43">
+        <v>3</v>
+      </c>
+      <c r="P43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>337</v>
+      </c>
+      <c r="C44" s="1">
+        <v>63</v>
+      </c>
+      <c r="D44">
+        <v>16</v>
+      </c>
+      <c r="E44">
+        <v>17</v>
+      </c>
+      <c r="F44">
+        <v>433</v>
+      </c>
+      <c r="G44">
+        <v>50</v>
+      </c>
+      <c r="H44">
+        <v>16</v>
+      </c>
+      <c r="I44">
+        <v>32</v>
+      </c>
+      <c r="J44">
+        <v>34</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>205</v>
+      </c>
+      <c r="M44">
+        <v>123</v>
+      </c>
+      <c r="N44">
+        <v>312</v>
+      </c>
+      <c r="O44">
+        <v>11</v>
+      </c>
+      <c r="P44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>15</v>
+      </c>
+      <c r="C45" s="1">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>22</v>
+      </c>
+      <c r="G45" t="s">
+        <v>66</v>
+      </c>
+      <c r="H45" t="s">
+        <v>66</v>
+      </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>10</v>
+      </c>
+      <c r="M45">
+        <v>4</v>
+      </c>
+      <c r="N45">
+        <v>14</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>5</v>
+      </c>
+      <c r="G46" t="s">
+        <v>66</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46" t="s">
+        <v>66</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46" t="s">
+        <v>66</v>
+      </c>
+      <c r="M46" t="s">
+        <v>66</v>
+      </c>
+      <c r="N46">
+        <v>3</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>61</v>
       </c>
-      <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>7</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>10</v>
+      </c>
+      <c r="G47" t="s">
+        <v>66</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47" t="s">
+        <v>66</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>3</v>
+      </c>
+      <c r="M47">
+        <v>3</v>
+      </c>
+      <c r="N47">
+        <v>7</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>86</v>
+      </c>
+      <c r="C48" s="1">
+        <v>13</v>
+      </c>
+      <c r="D48">
+        <v>7</v>
+      </c>
+      <c r="E48">
+        <v>5</v>
+      </c>
+      <c r="F48">
+        <v>111</v>
+      </c>
+      <c r="G48">
+        <v>11</v>
+      </c>
+      <c r="H48" t="s">
+        <v>66</v>
+      </c>
+      <c r="I48">
+        <v>8</v>
+      </c>
+      <c r="J48">
+        <v>4</v>
+      </c>
+      <c r="K48" t="s">
+        <v>66</v>
+      </c>
+      <c r="L48">
+        <v>48</v>
+      </c>
+      <c r="M48">
+        <v>26</v>
+      </c>
+      <c r="N48">
+        <v>81</v>
+      </c>
+      <c r="O48">
+        <v>5</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>63</v>
       </c>
-      <c r="C49" s="1"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>7</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>10</v>
+      </c>
+      <c r="G49" t="s">
+        <v>66</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49" t="s">
+        <v>66</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>3</v>
+      </c>
+      <c r="M49">
+        <v>3</v>
+      </c>
+      <c r="N49">
+        <v>7</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>64</v>
       </c>
-      <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>45</v>
+      </c>
+      <c r="C50" s="1">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>50</v>
+      </c>
+      <c r="G50">
+        <v>3</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50" t="s">
+        <v>66</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>35</v>
+      </c>
+      <c r="M50">
+        <v>11</v>
+      </c>
+      <c r="N50">
+        <v>43</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="1"/>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1">
+        <v>4</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>6</v>
+      </c>
+      <c r="G51">
+        <v>4</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>3</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51" t="s">
+        <v>66</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51" t="s">
+        <v>66</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Full Data - from Bereket, Doug, Brad
</commit_message>
<xml_diff>
--- a/data-v2.xlsx
+++ b/data-v2.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="67">
   <si>
     <t>state</t>
   </si>
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1567,97 +1567,758 @@
       <c r="O20">
         <v>0</v>
       </c>
-      <c r="P20" t="s">
-        <v>66</v>
+      <c r="P20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="B21">
+        <v>93</v>
+      </c>
+      <c r="C21" s="1">
+        <v>17</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>118</v>
+      </c>
+      <c r="G21">
+        <v>15</v>
+      </c>
+      <c r="H21" t="s">
+        <v>66</v>
+      </c>
+      <c r="I21">
+        <v>11</v>
+      </c>
+      <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>59</v>
+      </c>
+      <c r="M21">
+        <v>29</v>
+      </c>
+      <c r="N21">
+        <v>87</v>
+      </c>
+      <c r="O21" t="s">
+        <v>66</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="B22">
+        <v>51</v>
+      </c>
+      <c r="C22" s="1">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>6</v>
+      </c>
+      <c r="F22">
+        <v>62</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22" t="s">
+        <v>66</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
+      </c>
+      <c r="J22" t="s">
+        <v>66</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>36</v>
+      </c>
+      <c r="M22">
+        <v>17</v>
+      </c>
+      <c r="N22">
+        <v>45</v>
+      </c>
+      <c r="O22">
+        <v>5</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="B23">
+        <v>122</v>
+      </c>
+      <c r="C23" s="1">
+        <v>18</v>
+      </c>
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23">
+        <v>152</v>
+      </c>
+      <c r="G23">
+        <v>16</v>
+      </c>
+      <c r="H23" t="s">
+        <v>66</v>
+      </c>
+      <c r="I23">
+        <v>9</v>
+      </c>
+      <c r="J23">
+        <v>10</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>66</v>
+      </c>
+      <c r="M23">
+        <v>48</v>
+      </c>
+      <c r="N23">
+        <v>107</v>
+      </c>
+      <c r="O23">
+        <v>6</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="1"/>
+      <c r="B24">
+        <v>27</v>
+      </c>
+      <c r="C24" s="1">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>36</v>
+      </c>
+      <c r="G24">
+        <v>8</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>5</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>18</v>
+      </c>
+      <c r="M24">
+        <v>10</v>
+      </c>
+      <c r="N24">
+        <v>25</v>
+      </c>
+      <c r="O24" t="s">
+        <v>66</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="1"/>
+      <c r="B25">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>36</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25" t="s">
+        <v>66</v>
+      </c>
+      <c r="I25" t="s">
+        <v>66</v>
+      </c>
+      <c r="J25">
+        <v>3</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>18</v>
+      </c>
+      <c r="M25">
+        <v>7</v>
+      </c>
+      <c r="N25">
+        <v>24</v>
+      </c>
+      <c r="O25" t="s">
+        <v>66</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="1"/>
+      <c r="B26">
+        <v>58</v>
+      </c>
+      <c r="C26" s="1">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>67</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26" t="s">
+        <v>66</v>
+      </c>
+      <c r="I26">
+        <v>4</v>
+      </c>
+      <c r="J26" t="s">
+        <v>66</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>36</v>
+      </c>
+      <c r="M26">
+        <v>20</v>
+      </c>
+      <c r="N26">
+        <v>54</v>
+      </c>
+      <c r="O26">
+        <v>3</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="1"/>
+      <c r="B27">
+        <v>11</v>
+      </c>
+      <c r="C27" s="1">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>19</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>66</v>
+      </c>
+      <c r="J27">
+        <v>3</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>10</v>
+      </c>
+      <c r="M27" t="s">
+        <v>66</v>
+      </c>
+      <c r="N27">
+        <v>11</v>
+      </c>
+      <c r="O27" t="s">
+        <v>66</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="B28">
+        <v>14</v>
+      </c>
+      <c r="C28" s="1">
+        <v>7</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>24</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
+      </c>
+      <c r="H28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I28" t="s">
+        <v>66</v>
+      </c>
+      <c r="J28">
+        <v>5</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>7</v>
+      </c>
+      <c r="M28">
+        <v>6</v>
+      </c>
+      <c r="N28">
+        <v>14</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="1"/>
+      <c r="B29">
+        <v>114</v>
+      </c>
+      <c r="C29" s="1">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <v>133</v>
+      </c>
+      <c r="G29">
+        <v>10</v>
+      </c>
+      <c r="H29" t="s">
+        <v>66</v>
+      </c>
+      <c r="I29">
+        <v>5</v>
+      </c>
+      <c r="J29">
+        <v>7</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>85</v>
+      </c>
+      <c r="M29">
+        <v>31</v>
+      </c>
+      <c r="N29">
+        <v>107</v>
+      </c>
+      <c r="O29">
+        <v>6</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30" s="1">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>12</v>
+      </c>
+      <c r="G30">
+        <v>3</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>66</v>
+      </c>
+      <c r="J30" t="s">
+        <v>66</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>7</v>
+      </c>
+      <c r="M30" t="s">
+        <v>66</v>
+      </c>
+      <c r="N30">
+        <v>7</v>
+      </c>
+      <c r="O30" t="s">
+        <v>66</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="1"/>
+      <c r="B31">
+        <v>139</v>
+      </c>
+      <c r="C31" s="1">
+        <v>13</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <v>13</v>
+      </c>
+      <c r="F31">
+        <v>169</v>
+      </c>
+      <c r="G31">
+        <v>13</v>
+      </c>
+      <c r="H31" t="s">
+        <v>66</v>
+      </c>
+      <c r="I31">
+        <v>8</v>
+      </c>
+      <c r="J31">
+        <v>6</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>57</v>
+      </c>
+      <c r="M31">
+        <v>75</v>
+      </c>
+      <c r="N31">
+        <v>129</v>
+      </c>
+      <c r="O31">
+        <v>3</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="1"/>
+      <c r="B32">
+        <v>22</v>
+      </c>
+      <c r="C32" s="1">
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>28</v>
+      </c>
+      <c r="G32">
+        <v>3</v>
+      </c>
+      <c r="H32" t="s">
+        <v>66</v>
+      </c>
+      <c r="I32">
+        <v>3</v>
+      </c>
+      <c r="J32">
+        <v>4</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>14</v>
+      </c>
+      <c r="M32">
+        <v>8</v>
+      </c>
+      <c r="N32">
+        <v>16</v>
+      </c>
+      <c r="O32">
+        <v>4</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="1"/>
+      <c r="B33">
+        <v>217</v>
+      </c>
+      <c r="C33" s="1">
+        <v>39</v>
+      </c>
+      <c r="D33">
+        <v>15</v>
+      </c>
+      <c r="E33">
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>281</v>
+      </c>
+      <c r="G33">
+        <v>27</v>
+      </c>
+      <c r="H33">
+        <v>6</v>
+      </c>
+      <c r="I33">
+        <v>26</v>
+      </c>
+      <c r="J33">
+        <v>15</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>141</v>
+      </c>
+      <c r="M33">
+        <v>69</v>
+      </c>
+      <c r="N33">
+        <v>199</v>
+      </c>
+      <c r="O33">
+        <v>4</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="1"/>
+      <c r="B34">
+        <v>78</v>
+      </c>
+      <c r="C34" s="1">
+        <v>22</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <v>110</v>
+      </c>
+      <c r="G34">
+        <v>19</v>
+      </c>
+      <c r="H34" t="s">
+        <v>66</v>
+      </c>
+      <c r="I34">
+        <v>11</v>
+      </c>
+      <c r="J34">
+        <v>13</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>48</v>
+      </c>
+      <c r="M34">
+        <v>31</v>
+      </c>
+      <c r="N34">
+        <v>70</v>
+      </c>
+      <c r="O34">
+        <v>4</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>49</v>
+      </c>
+      <c r="B35">
+        <v>15</v>
+      </c>
+      <c r="C35" s="1">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>19</v>
+      </c>
+      <c r="G35">
+        <v>3</v>
+      </c>
+      <c r="H35" t="s">
+        <v>66</v>
+      </c>
+      <c r="I35">
+        <v>3</v>
+      </c>
+      <c r="J35" t="s">
+        <v>66</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>6</v>
+      </c>
+      <c r="M35">
+        <v>8</v>
+      </c>
+      <c r="N35">
+        <v>15</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>